<commit_message>
Updated blank correction,. inputs
</commit_message>
<xml_diff>
--- a/mad_test_3/AB11-2_AB13-2_reduction.xlsx
+++ b/mad_test_3/AB11-2_AB13-2_reduction.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr showInkAnnotation="0" updateLinks="never" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mitprod-my.sharepoint.com/personal/tigerb_mit_edu/Documents/Documents/GitHub/U_Th_dating/mad_test_3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{7A807CF7-B9A6-419F-A534-2A04A4174124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9AD11D99-C816-49D9-B6A4-19CCEF17915A}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{7A807CF7-B9A6-419F-A534-2A04A4174124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18E99531-3335-4D5B-ACCE-2048C1CA5E54}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="19320" windowHeight="11400" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -4368,7 +4368,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4493,6 +4493,7 @@
     <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="173" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4505,7 +4506,7 @@
     <xf numFmtId="174" fontId="22" fillId="0" borderId="0" xfId="1203" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1497">
     <cellStyle name="Bad" xfId="1267" builtinId="27"/>
@@ -6049,21 +6050,21 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -6589,6 +6590,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -8035,7 +8040,7 @@
       <c r="S25" s="38"/>
       <c r="T25" s="38"/>
     </row>
-    <row r="26" spans="1:20" ht="16.5">
+    <row r="26" spans="1:20">
       <c r="A26" s="71" t="s">
         <v>155</v>
       </c>
@@ -8057,7 +8062,7 @@
       <c r="S26" s="38"/>
       <c r="T26" s="38"/>
     </row>
-    <row r="27" spans="1:20" ht="16.5">
+    <row r="27" spans="1:20">
       <c r="A27" s="68" t="s">
         <v>152</v>
       </c>
@@ -8077,7 +8082,7 @@
       <c r="O27" s="39"/>
       <c r="P27" s="39"/>
     </row>
-    <row r="28" spans="1:20" ht="18">
+    <row r="28" spans="1:20" ht="16.149999999999999">
       <c r="A28" s="68" t="s">
         <v>161</v>
       </c>
@@ -8097,7 +8102,7 @@
       <c r="O28" s="39"/>
       <c r="P28" s="39"/>
     </row>
-    <row r="29" spans="1:20" ht="16.5">
+    <row r="29" spans="1:20">
       <c r="A29" s="68" t="s">
         <v>202</v>
       </c>
@@ -8117,7 +8122,7 @@
       <c r="O29" s="39"/>
       <c r="P29" s="39"/>
     </row>
-    <row r="30" spans="1:20" ht="16.5">
+    <row r="30" spans="1:20" ht="16.149999999999999">
       <c r="A30" s="68" t="s">
         <v>153</v>
       </c>
@@ -8137,7 +8142,7 @@
       <c r="O30" s="39"/>
       <c r="P30" s="39"/>
     </row>
-    <row r="31" spans="1:20" ht="16.5">
+    <row r="31" spans="1:20">
       <c r="A31" s="69" t="s">
         <v>164</v>
       </c>
@@ -8157,7 +8162,7 @@
       <c r="O31" s="39"/>
       <c r="P31" s="39"/>
     </row>
-    <row r="32" spans="1:20" ht="16.5">
+    <row r="32" spans="1:20">
       <c r="A32" s="70" t="s">
         <v>154</v>
       </c>
@@ -8192,8 +8197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CA65"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -8294,37 +8299,37 @@
       <c r="AE2" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="BE2" s="98" t="s">
+      <c r="BE2" s="99" t="s">
         <v>240</v>
       </c>
-      <c r="BF2" s="98"/>
-      <c r="BG2" s="98"/>
-      <c r="BH2" s="98" t="s">
+      <c r="BF2" s="99"/>
+      <c r="BG2" s="99"/>
+      <c r="BH2" s="99" t="s">
         <v>241</v>
       </c>
-      <c r="BI2" s="98"/>
-      <c r="BJ2" s="98"/>
-      <c r="BK2" s="98" t="s">
+      <c r="BI2" s="99"/>
+      <c r="BJ2" s="99"/>
+      <c r="BK2" s="99" t="s">
         <v>247</v>
       </c>
-      <c r="BL2" s="98"/>
-      <c r="BM2" s="98"/>
-      <c r="BN2" s="98" t="s">
+      <c r="BL2" s="99"/>
+      <c r="BM2" s="99"/>
+      <c r="BN2" s="99" t="s">
         <v>248</v>
       </c>
-      <c r="BO2" s="98"/>
-      <c r="BP2" s="98"/>
+      <c r="BO2" s="99"/>
+      <c r="BP2" s="99"/>
       <c r="BQ2" s="83"/>
-      <c r="BR2" s="98" t="s">
+      <c r="BR2" s="99" t="s">
         <v>266</v>
       </c>
-      <c r="BS2" s="98"/>
-      <c r="BT2" s="98"/>
-      <c r="BU2" s="98" t="s">
+      <c r="BS2" s="99"/>
+      <c r="BT2" s="99"/>
+      <c r="BU2" s="99" t="s">
         <v>267</v>
       </c>
-      <c r="BV2" s="98"/>
-      <c r="BW2" s="98"/>
+      <c r="BV2" s="99"/>
+      <c r="BW2" s="99"/>
       <c r="BX2" s="83"/>
     </row>
     <row r="3" spans="1:79">
@@ -14046,7 +14051,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:79" ht="16.5" thickBot="1">
+    <row r="27" spans="1:79" ht="16.149999999999999" thickBot="1">
       <c r="A27" s="66"/>
       <c r="B27" s="66"/>
       <c r="C27" s="66" t="s">
@@ -16289,7 +16294,7 @@
       <selection activeCell="E9" sqref="E9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
-      <selection pane="bottomRight" activeCell="H18" sqref="H18"/>
+      <selection pane="bottomRight" activeCell="AO4" sqref="AO4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -16341,28 +16346,28 @@
         <v>133</v>
       </c>
       <c r="CN2" s="2"/>
-      <c r="CQ2" s="99" t="s">
+      <c r="CQ2" s="100" t="s">
         <v>240</v>
       </c>
-      <c r="CR2" s="99"/>
-      <c r="CS2" s="99"/>
-      <c r="CT2" s="99" t="s">
+      <c r="CR2" s="100"/>
+      <c r="CS2" s="100"/>
+      <c r="CT2" s="100" t="s">
         <v>241</v>
       </c>
-      <c r="CU2" s="99"/>
-      <c r="CV2" s="99"/>
-      <c r="CW2" s="99"/>
-      <c r="CY2" s="100" t="s">
+      <c r="CU2" s="100"/>
+      <c r="CV2" s="100"/>
+      <c r="CW2" s="100"/>
+      <c r="CY2" s="101" t="s">
         <v>0</v>
       </c>
-      <c r="CZ2" s="100"/>
-      <c r="DA2" s="100"/>
-      <c r="DB2" s="100" t="s">
+      <c r="CZ2" s="101"/>
+      <c r="DA2" s="101"/>
+      <c r="DB2" s="101" t="s">
         <v>4</v>
       </c>
-      <c r="DC2" s="100"/>
-      <c r="DD2" s="100"/>
-      <c r="DE2" s="100"/>
+      <c r="DC2" s="101"/>
+      <c r="DD2" s="101"/>
+      <c r="DE2" s="101"/>
     </row>
     <row r="3" spans="1:109">
       <c r="A3" t="s">
@@ -40107,7 +40112,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:BB53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="I4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E9" sqref="E9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
@@ -40157,26 +40162,26 @@
         <f>Constants!B26</f>
         <v>6.3883454641536821E-7</v>
       </c>
-      <c r="AP2" s="98" t="s">
+      <c r="AP2" s="99" t="s">
         <v>235</v>
       </c>
-      <c r="AQ2" s="98"/>
-      <c r="AR2" s="98"/>
-      <c r="AS2" s="99" t="s">
+      <c r="AQ2" s="99"/>
+      <c r="AR2" s="99"/>
+      <c r="AS2" s="100" t="s">
         <v>236</v>
       </c>
-      <c r="AT2" s="99"/>
-      <c r="AU2" s="99"/>
-      <c r="AW2" s="101" t="s">
+      <c r="AT2" s="100"/>
+      <c r="AU2" s="100"/>
+      <c r="AW2" s="102" t="s">
         <v>109</v>
       </c>
-      <c r="AX2" s="101"/>
-      <c r="AY2" s="101"/>
-      <c r="AZ2" s="100" t="s">
+      <c r="AX2" s="102"/>
+      <c r="AY2" s="102"/>
+      <c r="AZ2" s="101" t="s">
         <v>100</v>
       </c>
-      <c r="BA2" s="100"/>
-      <c r="BB2" s="100"/>
+      <c r="BA2" s="101"/>
+      <c r="BB2" s="101"/>
     </row>
     <row r="3" spans="1:54">
       <c r="A3" t="str">
@@ -40427,7 +40432,7 @@
         <f>IF(NOT(ISBLANK($J5)), IF((ABS($J4-$J6)/$J4)&gt;Constants!$B$31,"variable IC yield","OK"), "")</f>
         <v>OK</v>
       </c>
-      <c r="E5" s="49">
+      <c r="E5" s="103">
         <f>AK5</f>
         <v>0.6387236237584758</v>
       </c>
@@ -40435,7 +40440,7 @@
         <f>AL5</f>
         <v>0.59250287514828237</v>
       </c>
-      <c r="G5" s="49">
+      <c r="G5" s="103">
         <f>AM5</f>
         <v>1.0804664906155287E-4</v>
       </c>
@@ -45164,6 +45169,19 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
+          <x14:cfRule type="expression" priority="15" id="{069C5E89-77CD-AB4F-B109-7C367E52547F}">
+            <xm:f>AND(NOT(ISBLANK(B5)),AR5&gt;(Constants!$B$38*AQ5))</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C6500"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFEB9C"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
           <x14:cfRule type="expression" priority="17" id="{EB4CD11B-4043-0640-BA98-EB4DF1B16716}">
             <xm:f>AND(NOT(ISBLANK(B5)),(AR5-AQ5)&gt;Constants!$B$37)</xm:f>
             <x14:dxf>
@@ -45173,19 +45191,6 @@
               <fill>
                 <patternFill>
                   <bgColor rgb="FFC6EFCE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="expression" priority="15" id="{069C5E89-77CD-AB4F-B109-7C367E52547F}">
-            <xm:f>AND(NOT(ISBLANK(B5)),AR5&gt;(Constants!$B$38*AQ5))</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF9C6500"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFEB9C"/>
                 </patternFill>
               </fill>
             </x14:dxf>
@@ -45351,7 +45356,7 @@
         <v>9.170520780000001E-6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="16.5" thickBot="1">
+    <row r="9" spans="1:11" ht="16.149999999999999" thickBot="1">
       <c r="A9" s="25" t="s">
         <v>53</v>
       </c>
@@ -45361,7 +45366,7 @@
       <c r="C9" s="26"/>
       <c r="D9" s="26"/>
     </row>
-    <row r="10" spans="1:11" ht="16.5" thickBot="1"/>
+    <row r="10" spans="1:11" ht="16.149999999999999" thickBot="1"/>
     <row r="11" spans="1:11">
       <c r="A11" s="6" t="s">
         <v>24</v>
@@ -45443,7 +45448,7 @@
         <v>1.7442466578521214E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="16.5" thickBot="1">
+    <row r="14" spans="1:11" ht="16.149999999999999" thickBot="1">
       <c r="A14" s="17" t="s">
         <v>37</v>
       </c>
@@ -45479,7 +45484,7 @@
         <v>5.6732610254575369E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="16.5" thickBot="1"/>
+    <row r="15" spans="1:11" ht="16.149999999999999" thickBot="1"/>
     <row r="16" spans="1:11">
       <c r="A16" s="6" t="s">
         <v>40</v>
@@ -45520,7 +45525,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="16.5" thickBot="1">
+    <row r="19" spans="1:14" ht="16.149999999999999" thickBot="1">
       <c r="A19" s="21" t="s">
         <v>51</v>
       </c>
@@ -45574,7 +45579,7 @@
         <v>2.3386571119731001E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="16.5" thickBot="1">
+    <row r="21" spans="1:14" ht="16.149999999999999" thickBot="1">
       <c r="A21" s="21"/>
       <c r="B21" t="s">
         <v>56</v>
@@ -45608,11 +45613,11 @@
       <c r="M21" s="18">
         <v>4.9678648462572098E-2</v>
       </c>
-      <c r="N21" s="102">
+      <c r="N21" s="98">
         <v>6.2828101662080203E-6</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="16.5" thickBot="1">
+    <row r="22" spans="1:14" ht="16.149999999999999" thickBot="1">
       <c r="A22" s="29"/>
       <c r="B22" s="18" t="s">
         <v>84</v>
@@ -46626,7 +46631,7 @@
   <dimension ref="A1:Q38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -48396,7 +48401,7 @@
   <dimension ref="A1:S28"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>

</xml_diff>